<commit_message>
Second revision NHESS paper
</commit_message>
<xml_diff>
--- a/input_data/Mapping_maxdamage_curves4.xlsx
+++ b/input_data/Mapping_maxdamage_curves4.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D339D8A-AD4F-4C85-9DF3-410098B4D000}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41E55154-98EF-436E-88B2-8568FB12DC27}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="45972" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Max_damages" sheetId="5" r:id="rId1"/>
@@ -571,7 +571,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="142">
   <si>
     <t>OSM_highwayKey_value</t>
   </si>
@@ -11120,34 +11120,34 @@
       <selection activeCell="H5" sqref="H5:M12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.84375" customWidth="1"/>
+    <col min="4" max="4" width="12.53515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11.28515625" customWidth="1"/>
-    <col min="15" max="15" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.7109375" customWidth="1"/>
-    <col min="17" max="18" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.7109375" customWidth="1"/>
-    <col min="20" max="20" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.42578125" customWidth="1"/>
-    <col min="24" max="27" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.3046875" customWidth="1"/>
+    <col min="15" max="15" width="10.15234375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.69140625" customWidth="1"/>
+    <col min="17" max="18" width="10.15234375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.69140625" customWidth="1"/>
+    <col min="20" max="20" width="10.15234375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.15234375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.3828125" customWidth="1"/>
+    <col min="24" max="27" width="11.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.4">
       <c r="C1" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.4">
       <c r="B2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.4">
       <c r="B3" s="1" t="s">
         <v>80</v>
       </c>
@@ -11161,7 +11161,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.4">
       <c r="B4" t="s">
         <v>53</v>
       </c>
@@ -11233,7 +11233,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>100</v>
       </c>
@@ -11317,7 +11317,7 @@
         <v>35000000</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>100</v>
       </c>
@@ -11401,7 +11401,7 @@
         <v>7500000</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.4">
       <c r="C7" t="s">
         <v>32</v>
       </c>
@@ -11482,7 +11482,7 @@
         <v>6000000</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.4">
       <c r="C8" t="s">
         <v>36</v>
       </c>
@@ -11563,7 +11563,7 @@
         <v>3000000</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.4">
       <c r="C9" t="s">
         <v>29</v>
       </c>
@@ -11644,7 +11644,7 @@
         <v>1350000</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.4">
       <c r="C10" t="s">
         <v>3</v>
       </c>
@@ -11725,7 +11725,7 @@
         <v>675000</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.4">
       <c r="C11" t="s">
         <v>8</v>
       </c>
@@ -11806,7 +11806,7 @@
         <v>112500</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.4">
       <c r="C12" t="s">
         <v>122</v>
       </c>
@@ -11886,16 +11886,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.4">
       <c r="P16" s="5"/>
     </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="6:6" x14ac:dyDescent="0.4">
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="6:6" x14ac:dyDescent="0.4">
       <c r="F18" s="5"/>
     </row>
   </sheetData>
@@ -11908,16 +11908,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="I41" sqref="I41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -11925,7 +11925,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -11933,7 +11933,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -11941,7 +11941,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -11949,7 +11949,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -11957,7 +11957,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -11965,7 +11965,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -11973,7 +11973,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -11981,7 +11981,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -11989,7 +11989,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -11997,7 +11997,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -12005,7 +12005,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -12013,7 +12013,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -12021,7 +12021,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -12029,7 +12029,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -12037,7 +12037,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -12045,7 +12045,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -12053,7 +12053,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -12061,7 +12061,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -12069,7 +12069,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -12077,7 +12077,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -12085,7 +12085,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -12093,7 +12093,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -12101,7 +12101,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -12109,7 +12109,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -12117,7 +12117,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>28</v>
       </c>
@@ -12125,7 +12125,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>30</v>
       </c>
@@ -12133,7 +12133,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>31</v>
       </c>
@@ -12141,7 +12141,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>32</v>
       </c>
@@ -12149,7 +12149,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -12157,7 +12157,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>34</v>
       </c>
@@ -12165,7 +12165,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
         <v>35</v>
       </c>
@@ -12173,7 +12173,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>36</v>
       </c>
@@ -12181,7 +12181,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>37</v>
       </c>
@@ -12189,7 +12189,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>38</v>
       </c>
@@ -12197,7 +12197,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
         <v>39</v>
       </c>
@@ -12205,7 +12205,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
         <v>29</v>
       </c>
@@ -12213,7 +12213,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
         <v>40</v>
       </c>
@@ -12221,7 +12221,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
         <v>8</v>
       </c>
@@ -12229,7 +12229,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
         <v>41</v>
       </c>
@@ -12237,7 +12237,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
         <v>42</v>
       </c>
@@ -12245,7 +12245,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
         <v>43</v>
       </c>
@@ -12253,7 +12253,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
         <v>44</v>
       </c>
@@ -12261,7 +12261,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
         <v>45</v>
       </c>
@@ -12269,7 +12269,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
         <v>46</v>
       </c>
@@ -12277,7 +12277,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
         <v>47</v>
       </c>
@@ -12285,7 +12285,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
         <v>123</v>
       </c>
@@ -12293,7 +12293,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
         <v>124</v>
       </c>
@@ -12301,7 +12301,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
         <v>125</v>
       </c>
@@ -12309,7 +12309,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A50" t="s">
         <v>126</v>
       </c>
@@ -12317,7 +12317,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A51" t="s">
         <v>131</v>
       </c>
@@ -12335,26 +12335,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:O20"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5:M9"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="8.85546875" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" customWidth="1"/>
+    <col min="2" max="2" width="8.84375" customWidth="1"/>
+    <col min="3" max="3" width="9.3828125" customWidth="1"/>
+    <col min="4" max="4" width="9.53515625" customWidth="1"/>
+    <col min="5" max="5" width="9.69140625" customWidth="1"/>
+    <col min="7" max="7" width="9.3828125" customWidth="1"/>
+    <col min="9" max="9" width="10.15234375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" s="7" t="s">
         <v>60</v>
       </c>
@@ -12380,7 +12380,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4" s="1"/>
       <c r="B4" t="s">
         <v>58</v>
@@ -12418,8 +12418,14 @@
       <c r="M4" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N4" t="s">
+        <v>58</v>
+      </c>
+      <c r="O4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A5" s="1"/>
       <c r="B5" s="12">
         <f>Motorway_curves!B6</f>
@@ -12476,7 +12482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A6" s="1"/>
       <c r="B6" s="12">
         <f>Motorway_curves!B7</f>
@@ -12533,7 +12539,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A7" s="1"/>
       <c r="B7" s="12">
         <f>Motorway_curves!B8</f>
@@ -12590,7 +12596,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A8" s="1"/>
       <c r="B8" s="12">
         <f>Motorway_curves!B9</f>
@@ -12647,7 +12653,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A9" s="1"/>
       <c r="B9" s="12">
         <f>Motorway_curves!B10</f>
@@ -12704,7 +12710,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A10" s="1"/>
       <c r="B10" s="12">
         <f>Motorway_curves!B11</f>
@@ -12745,7 +12751,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A11" s="1"/>
       <c r="N11">
         <v>400</v>
@@ -12754,7 +12760,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A12" s="1"/>
       <c r="N12">
         <v>500</v>
@@ -12763,7 +12769,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
       <c r="N13">
         <v>600</v>
       </c>
@@ -12771,16 +12777,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A16" s="1"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -12799,24 +12805,24 @@
       <selection activeCell="B6" sqref="B6:L11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="8.85546875" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" customWidth="1"/>
-    <col min="9" max="9" width="9.42578125" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" customWidth="1"/>
+    <col min="2" max="2" width="8.84375" customWidth="1"/>
+    <col min="3" max="3" width="9.3828125" customWidth="1"/>
+    <col min="4" max="4" width="9.69140625" customWidth="1"/>
+    <col min="5" max="5" width="9.53515625" customWidth="1"/>
+    <col min="6" max="6" width="9.69140625" customWidth="1"/>
+    <col min="7" max="7" width="10.84375" customWidth="1"/>
+    <col min="9" max="9" width="9.3828125" customWidth="1"/>
+    <col min="12" max="12" width="10.15234375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A3" s="7" t="s">
         <v>60</v>
       </c>
@@ -12839,7 +12845,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.4">
       <c r="B4" t="s">
         <v>127</v>
       </c>
@@ -12862,7 +12868,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A5" s="1"/>
       <c r="B5" t="s">
         <v>58</v>
@@ -12895,7 +12901,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A6" s="1"/>
       <c r="B6" s="12">
         <v>0</v>
@@ -12934,7 +12940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A7" s="1"/>
       <c r="B7" s="12">
         <v>50</v>
@@ -12973,7 +12979,7 @@
         <v>2.0905923344947737E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A8" s="1"/>
       <c r="B8" s="12">
         <v>100</v>
@@ -13012,7 +13018,7 @@
         <v>3.5121951219512199E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A9" s="1"/>
       <c r="B9" s="12">
         <v>150</v>
@@ -13051,7 +13057,7 @@
         <v>4.5993031358885016E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A10" s="1"/>
       <c r="B10" s="12">
         <v>200</v>
@@ -13090,7 +13096,7 @@
         <v>5.4355400696864113E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A11" s="1"/>
       <c r="B11" s="12">
         <v>600</v>
@@ -13129,7 +13135,7 @@
         <v>6.6898954703832753E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A12" s="1"/>
       <c r="N12">
         <v>400</v>
@@ -13143,7 +13149,7 @@
         <v>7.526132404181185E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A13" s="1"/>
       <c r="N13">
         <v>500</v>
@@ -13157,7 +13163,7 @@
         <v>8.3623693379790948E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.4">
       <c r="N14">
         <v>600</v>
       </c>
@@ -13170,15 +13176,15 @@
         <v>8.3623693379790948E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A16" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A17" s="1"/>
       <c r="B17" t="str">
         <f t="shared" ref="B17:B24" si="2">B4</f>
@@ -13201,7 +13207,7 @@
         <v>C7 Huizinga</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A18" s="1"/>
       <c r="B18" t="str">
         <f t="shared" si="2"/>
@@ -13236,7 +13242,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.4">
       <c r="B19" s="13">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -13276,7 +13282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.4">
       <c r="B20" s="13">
         <f t="shared" si="2"/>
         <v>50</v>
@@ -13316,7 +13322,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.4">
       <c r="B21" s="13">
         <f t="shared" si="2"/>
         <v>100</v>
@@ -13356,7 +13362,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.4">
       <c r="B22" s="13">
         <f t="shared" si="2"/>
         <v>150</v>
@@ -13396,7 +13402,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.4">
       <c r="B23" s="13">
         <f t="shared" si="2"/>
         <v>200</v>
@@ -13436,7 +13442,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.4">
       <c r="B24" s="13">
         <f t="shared" si="2"/>
         <v>600</v>
@@ -13476,7 +13482,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.4">
       <c r="N25" s="8">
         <v>400</v>
       </c>
@@ -13484,7 +13490,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.4">
       <c r="N26" s="8">
         <v>500</v>
       </c>
@@ -13492,7 +13498,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.4">
       <c r="N27" s="8">
         <v>600</v>
       </c>
@@ -13500,12 +13506,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A35" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.4">
       <c r="B36" t="s">
         <v>58</v>
       </c>
@@ -13545,7 +13551,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.4">
       <c r="C37" t="s">
         <v>132</v>
       </c>
@@ -13578,7 +13584,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.4">
       <c r="B38">
         <f t="shared" ref="B38:B43" si="11">B6</f>
         <v>0</v>
@@ -13624,7 +13630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.4">
       <c r="B39">
         <f t="shared" si="11"/>
         <v>50</v>
@@ -13670,7 +13676,7 @@
         <v>300000</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.4">
       <c r="B40">
         <f t="shared" si="11"/>
         <v>100</v>
@@ -13716,7 +13722,7 @@
         <v>504000</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.4">
       <c r="B41">
         <f t="shared" si="11"/>
         <v>150</v>
@@ -13762,7 +13768,7 @@
         <v>660000</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.4">
       <c r="B42">
         <f t="shared" si="11"/>
         <v>200</v>
@@ -13808,7 +13814,7 @@
         <v>780000</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.4">
       <c r="B43">
         <f t="shared" si="11"/>
         <v>600</v>
@@ -13854,7 +13860,7 @@
         <v>960000</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.4">
       <c r="N44" s="13">
         <f t="shared" si="10"/>
         <v>400</v>
@@ -13864,7 +13870,7 @@
         <v>1080000</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.4">
       <c r="B45">
         <f>B13</f>
         <v>0</v>
@@ -13882,7 +13888,7 @@
         <v>1200000</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.4">
       <c r="N46" s="13">
         <f t="shared" si="10"/>
         <v>600</v>
@@ -13892,12 +13898,12 @@
         <v>1200000</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.4">
       <c r="N51" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.4">
       <c r="N52" t="s">
         <v>65</v>
       </c>
@@ -13908,7 +13914,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.4">
       <c r="N53" t="s">
         <v>67</v>
       </c>
@@ -13919,7 +13925,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.4">
       <c r="N54" t="s">
         <v>69</v>
       </c>
@@ -13930,7 +13936,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.4">
       <c r="N55" t="s">
         <v>70</v>
       </c>
@@ -13942,7 +13948,7 @@
         <v>1200000</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -13963,22 +13969,22 @@
       <selection activeCell="K49" sqref="K49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="8.85546875" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" customWidth="1"/>
+    <col min="2" max="2" width="8.84375" customWidth="1"/>
+    <col min="3" max="3" width="9.3828125" customWidth="1"/>
+    <col min="4" max="4" width="9.69140625" customWidth="1"/>
+    <col min="5" max="5" width="9.53515625" customWidth="1"/>
+    <col min="6" max="6" width="9.69140625" customWidth="1"/>
+    <col min="7" max="7" width="10.84375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A3" s="7" t="s">
         <v>60</v>
       </c>
@@ -13995,7 +14001,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
       <c r="B4" t="s">
         <v>98</v>
       </c>
@@ -14012,7 +14018,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A5" s="1"/>
       <c r="B5" t="s">
         <v>58</v>
@@ -14033,7 +14039,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A6" s="1"/>
       <c r="B6" s="12">
         <v>0</v>
@@ -14059,7 +14065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A7" s="1"/>
       <c r="B7" s="12">
         <v>50</v>
@@ -14085,7 +14091,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A8" s="1"/>
       <c r="B8" s="12">
         <v>100</v>
@@ -14111,7 +14117,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A9" s="1"/>
       <c r="B9" s="12">
         <v>200</v>
@@ -14137,7 +14143,7 @@
         <v>9.166666666666666E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A10" s="1"/>
       <c r="B10" s="12">
         <v>600</v>
@@ -14163,7 +14169,7 @@
         <v>0.10833333333333334</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A11" s="1"/>
       <c r="H11">
         <v>300</v>
@@ -14177,7 +14183,7 @@
         <v>0.13333333333333333</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A12" s="1"/>
       <c r="H12">
         <v>400</v>
@@ -14191,7 +14197,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A13" s="1"/>
       <c r="H13">
         <v>500</v>
@@ -14205,7 +14211,7 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
       <c r="H14">
         <v>600</v>
       </c>
@@ -14218,15 +14224,15 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A16" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A17" s="1"/>
       <c r="B17" t="str">
         <f t="shared" ref="B17:B23" si="0">B4</f>
@@ -14241,7 +14247,7 @@
         <v>Huizinga</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A18" s="1"/>
       <c r="B18" t="str">
         <f t="shared" si="0"/>
@@ -14262,7 +14268,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
       <c r="B19" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -14286,7 +14292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
       <c r="B20" s="13">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -14310,7 +14316,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
       <c r="B21" s="13">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -14334,7 +14340,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
       <c r="B22" s="13">
         <f t="shared" si="0"/>
         <v>200</v>
@@ -14358,7 +14364,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.4">
       <c r="B23" s="13">
         <f t="shared" si="0"/>
         <v>600</v>
@@ -14382,7 +14388,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.4">
       <c r="H24" s="8">
         <v>300</v>
       </c>
@@ -14390,7 +14396,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.4">
       <c r="H25" s="8">
         <v>400</v>
       </c>
@@ -14398,7 +14404,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.4">
       <c r="H26" s="8">
         <v>500</v>
       </c>
@@ -14406,7 +14412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.4">
       <c r="H27" s="8">
         <v>600</v>
       </c>
@@ -14414,12 +14420,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A35" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.4">
       <c r="B36" t="s">
         <v>58</v>
       </c>
@@ -14443,7 +14449,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.4">
       <c r="C37" t="s">
         <v>55</v>
       </c>
@@ -14464,7 +14470,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.4">
       <c r="B38">
         <v>0</v>
       </c>
@@ -14493,7 +14499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.4">
       <c r="B39">
         <v>50</v>
       </c>
@@ -14522,7 +14528,7 @@
         <v>62500</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.4">
       <c r="B40">
         <v>100</v>
       </c>
@@ -14551,7 +14557,7 @@
         <v>105000</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.4">
       <c r="B41">
         <v>200</v>
       </c>
@@ -14580,7 +14586,7 @@
         <v>137500</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.4">
       <c r="B42">
         <v>600</v>
       </c>
@@ -14609,7 +14615,7 @@
         <v>162500</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.4">
       <c r="H43" s="13">
         <f t="shared" si="3"/>
         <v>300</v>
@@ -14619,7 +14625,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.4">
       <c r="H44" s="13">
         <f t="shared" si="3"/>
         <v>400</v>
@@ -14629,7 +14635,7 @@
         <v>225000</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.4">
       <c r="D45" s="11"/>
       <c r="H45" s="13">
         <f t="shared" si="3"/>
@@ -14640,7 +14646,7 @@
         <v>250000</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.4">
       <c r="H46" s="13">
         <f t="shared" si="3"/>
         <v>600</v>
@@ -14650,12 +14656,12 @@
         <v>250000</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.4">
       <c r="H51" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.4">
       <c r="H52" t="s">
         <v>65</v>
       </c>
@@ -14666,7 +14672,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.4">
       <c r="H53" t="s">
         <v>67</v>
       </c>
@@ -14677,7 +14683,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.4">
       <c r="H54" t="s">
         <v>69</v>
       </c>
@@ -14688,7 +14694,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.4">
       <c r="H55" t="s">
         <v>88</v>
       </c>
@@ -14700,12 +14706,12 @@
         <v>250000</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A59" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.4">
       <c r="B60" t="s">
         <v>58</v>
       </c>
@@ -14729,7 +14735,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.4">
       <c r="C61" t="s">
         <v>55</v>
       </c>
@@ -14749,7 +14755,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.4">
       <c r="B62">
         <v>0</v>
       </c>
@@ -14778,7 +14784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.4">
       <c r="B63">
         <v>50</v>
       </c>
@@ -14807,7 +14813,7 @@
         <v>48000</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.4">
       <c r="B64">
         <v>100</v>
       </c>
@@ -14836,7 +14842,7 @@
         <v>80640</v>
       </c>
     </row>
-    <row r="65" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B65">
         <v>200</v>
       </c>
@@ -14865,7 +14871,7 @@
         <v>105600.00000000001</v>
       </c>
     </row>
-    <row r="66" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B66">
         <v>600</v>
       </c>
@@ -14894,7 +14900,7 @@
         <v>124800</v>
       </c>
     </row>
-    <row r="67" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:10" x14ac:dyDescent="0.4">
       <c r="H67" s="13">
         <f t="shared" si="5"/>
         <v>300</v>
@@ -14904,7 +14910,7 @@
         <v>153600</v>
       </c>
     </row>
-    <row r="68" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:10" x14ac:dyDescent="0.4">
       <c r="H68" s="13">
         <f t="shared" si="5"/>
         <v>400</v>
@@ -14914,7 +14920,7 @@
         <v>172800</v>
       </c>
     </row>
-    <row r="69" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:10" x14ac:dyDescent="0.4">
       <c r="D69" s="11"/>
       <c r="H69" s="13">
         <f t="shared" si="5"/>
@@ -14925,7 +14931,7 @@
         <v>192000</v>
       </c>
     </row>
-    <row r="70" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:10" x14ac:dyDescent="0.4">
       <c r="H70" s="13">
         <f t="shared" si="5"/>
         <v>600</v>
@@ -14935,12 +14941,12 @@
         <v>192000</v>
       </c>
     </row>
-    <row r="73" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:10" x14ac:dyDescent="0.4">
       <c r="H73" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="74" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:10" x14ac:dyDescent="0.4">
       <c r="H74" t="s">
         <v>65</v>
       </c>
@@ -14951,7 +14957,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="75" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:10" x14ac:dyDescent="0.4">
       <c r="H75" t="s">
         <v>67</v>
       </c>
@@ -14962,7 +14968,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="76" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:10" x14ac:dyDescent="0.4">
       <c r="H76" t="s">
         <v>69</v>
       </c>
@@ -14973,7 +14979,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="77" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:10" x14ac:dyDescent="0.4">
       <c r="H77" t="s">
         <v>89</v>
       </c>
@@ -15001,14 +15007,14 @@
       <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" customWidth="1"/>
-    <col min="3" max="8" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.3828125" customWidth="1"/>
+    <col min="2" max="2" width="11.3828125" customWidth="1"/>
+    <col min="3" max="8" width="12.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>54</v>
       </c>
@@ -15031,7 +15037,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" s="19" t="s">
         <v>43</v>
       </c>
@@ -15060,7 +15066,7 @@
         <v>750000</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" s="19" t="s">
         <v>42</v>
       </c>
@@ -15089,7 +15095,7 @@
         <v>650000</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" s="19" t="s">
         <v>32</v>
       </c>
@@ -15118,7 +15124,7 @@
         <v>575000</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="19" t="s">
         <v>36</v>
       </c>
@@ -15147,7 +15153,7 @@
         <v>550000</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" s="19" t="s">
         <v>29</v>
       </c>
@@ -15176,7 +15182,7 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7" s="19" t="s">
         <v>8</v>
       </c>
@@ -15205,7 +15211,7 @@
         <v>450000</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" s="19" t="s">
         <v>3</v>
       </c>
@@ -15248,14 +15254,14 @@
       <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B3" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B4" t="s">
         <v>54</v>
       </c>
@@ -15281,7 +15287,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B5" s="19" t="s">
         <v>43</v>
       </c>
@@ -15310,7 +15316,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B6" s="19" t="s">
         <v>42</v>
       </c>
@@ -15333,7 +15339,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B7" s="19" t="s">
         <v>32</v>
       </c>
@@ -15356,7 +15362,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B8" s="19" t="s">
         <v>36</v>
       </c>
@@ -15379,7 +15385,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B9" s="19" t="s">
         <v>29</v>
       </c>
@@ -15402,7 +15408,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B10" s="19" t="s">
         <v>8</v>
       </c>
@@ -15425,7 +15431,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B11" s="19" t="s">
         <v>3</v>
       </c>
@@ -15462,18 +15468,18 @@
       <selection activeCell="P6" sqref="P6:Z11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="3" max="5" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" customWidth="1"/>
-    <col min="8" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" customWidth="1"/>
+    <col min="3" max="5" width="14.15234375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.15234375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.15234375" customWidth="1"/>
+    <col min="8" max="9" width="10.84375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.69140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.84375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.15234375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.4">
       <c r="C2" t="s">
         <v>105</v>
       </c>
@@ -15500,7 +15506,7 @@
         <v>11.375</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.4">
       <c r="C3" s="21" t="s">
         <v>106</v>
       </c>
@@ -15537,7 +15543,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.4">
       <c r="B4" t="s">
         <v>104</v>
       </c>
@@ -15580,7 +15586,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.4">
       <c r="B5" t="s">
         <v>109</v>
       </c>
@@ -15635,7 +15641,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.4">
       <c r="P6" s="12">
         <v>0</v>
       </c>
@@ -15662,7 +15668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.4">
       <c r="C7" s="1" t="s">
         <v>113</v>
       </c>
@@ -15695,7 +15701,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.4">
       <c r="C8" s="7" t="s">
         <v>75</v>
       </c>
@@ -15746,7 +15752,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.4">
       <c r="B9" t="s">
         <v>104</v>
       </c>
@@ -15809,7 +15815,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.4">
       <c r="B10" t="s">
         <v>109</v>
       </c>
@@ -15872,7 +15878,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.4">
       <c r="B12" t="s">
         <v>115</v>
       </c>
@@ -15913,7 +15919,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.4">
       <c r="P13" t="s">
         <v>55</v>
       </c>
@@ -15921,7 +15927,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A14" s="1" t="s">
         <v>116</v>
       </c>
@@ -15935,7 +15941,7 @@
         <v>7500000</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>117</v>
       </c>
@@ -15944,7 +15950,7 @@
         <v>0.878</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.4">
       <c r="B16" t="s">
         <v>115</v>
       </c>
@@ -15982,7 +15988,7 @@
         <v>74.27879999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>119</v>
       </c>
@@ -16003,7 +16009,7 @@
         <v>74.27879999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>121</v>
       </c>
@@ -16016,7 +16022,7 @@
         <v>32.496974999999992</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.4">
       <c r="I23">
         <f ca="1">11.375*J4</f>
         <v>0.6256250000000001</v>
@@ -16026,7 +16032,7 @@
         <v>4.1291250000000002</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.4">
       <c r="I24">
         <f ca="1">11.375*K4</f>
         <v>6.8250000000000002</v>
@@ -16036,7 +16042,7 @@
         <v>19.11</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>120</v>
       </c>
@@ -16056,18 +16062,18 @@
       <selection activeCell="P18" sqref="P18:R19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="3" max="5" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" customWidth="1"/>
-    <col min="8" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" customWidth="1"/>
+    <col min="3" max="5" width="14.15234375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.15234375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.15234375" customWidth="1"/>
+    <col min="8" max="9" width="10.84375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.69140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.84375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.15234375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.4">
       <c r="C2" t="s">
         <v>105</v>
       </c>
@@ -16097,7 +16103,7 @@
         <v>11.375</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.4">
       <c r="C3" s="21" t="s">
         <v>106</v>
       </c>
@@ -16141,7 +16147,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.4">
       <c r="B4" t="s">
         <v>104</v>
       </c>
@@ -16191,7 +16197,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.4">
       <c r="B5" t="s">
         <v>109</v>
       </c>
@@ -16246,7 +16252,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.4">
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
       <c r="J6" s="10"/>
@@ -16277,7 +16283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.4">
       <c r="C7" s="1" t="s">
         <v>77</v>
       </c>
@@ -16314,7 +16320,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.4">
       <c r="B8" t="s">
         <v>104</v>
       </c>
@@ -16352,7 +16358,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.4">
       <c r="B9" t="s">
         <v>109</v>
       </c>
@@ -16397,7 +16403,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.4">
       <c r="B10" t="s">
         <v>136</v>
       </c>
@@ -16442,7 +16448,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.4">
       <c r="P11" s="12">
         <v>600</v>
       </c>
@@ -16469,7 +16475,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.4">
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
@@ -16480,12 +16486,12 @@
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.4">
       <c r="B13" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A14" s="1"/>
       <c r="B14" t="s">
         <v>138</v>
@@ -16496,7 +16502,7 @@
       <c r="P14" s="23"/>
       <c r="Q14" s="23"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.4">
       <c r="B15" t="s">
         <v>139</v>
       </c>
@@ -16504,7 +16510,7 @@
         <v>0.96250000000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.4">
       <c r="C16" s="24"/>
       <c r="D16" s="24"/>
       <c r="E16" s="24"/>
@@ -16515,7 +16521,7 @@
       <c r="J16" s="24"/>
       <c r="K16" s="24"/>
     </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:18" x14ac:dyDescent="0.4">
       <c r="C18" s="1" t="s">
         <v>77</v>
       </c>
@@ -16538,7 +16544,7 @@
         <v>2.6731249999999998</v>
       </c>
     </row>
-    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:18" x14ac:dyDescent="0.4">
       <c r="B19" t="s">
         <v>104</v>
       </c>
@@ -16566,7 +16572,7 @@
         <v>21.384999999999998</v>
       </c>
     </row>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:18" x14ac:dyDescent="0.4">
       <c r="B20" t="s">
         <v>109</v>
       </c>
@@ -16585,7 +16591,7 @@
         <v>21.384999999999998</v>
       </c>
     </row>
-    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:18" x14ac:dyDescent="0.4">
       <c r="B21" t="s">
         <v>136</v>
       </c>

</xml_diff>